<commit_message>
Adiciona relatorio 5 e modifica simulacao BBAS4
</commit_message>
<xml_diff>
--- a/d-4/5a_semana/BBAS4/simulacao_investimentos5BBAS4.xlsx
+++ b/d-4/5a_semana/BBAS4/simulacao_investimentos5BBAS4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiyom\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4EDE7004-F49B-4B29-B64F-D5F085CB1A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{54A4B6DA-5062-4942-8E79-83D7E189A792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1992-1998 (Parte 5)" sheetId="1" r:id="rId1"/>
@@ -930,8 +930,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000%"/>
-    <numFmt numFmtId="167" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1513,14 +1513,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="33" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="33" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="19" fillId="33" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="33" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="19" fillId="33" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="19" fillId="33" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="19" fillId="33" borderId="12" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -1880,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5423,8 +5423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2201CD4D-02EC-473D-B30F-626863316698}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5509,12 +5509,12 @@
         <v>765</v>
       </c>
       <c r="K2" s="6">
-        <f>J2</f>
-        <v>765</v>
+        <f>J2 + '1992-1998 (Parte 5)'!K73</f>
+        <v>1046114.6147274781</v>
       </c>
       <c r="L2" s="4">
         <f>K2*B2</f>
-        <v>749.69999999999993</v>
+        <v>1025192.3224329286</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="17" t="s">
@@ -5557,11 +5557,11 @@
       </c>
       <c r="K3" s="6">
         <f>K2+J3</f>
-        <v>1607.696629213483</v>
+        <v>1046957.3113566916</v>
       </c>
       <c r="L3" s="4">
         <f>K3*B3</f>
-        <v>1430.85</v>
+        <v>931792.00710745563</v>
       </c>
       <c r="N3" s="6"/>
       <c r="O3" s="12" t="s">
@@ -5569,11 +5569,11 @@
       </c>
       <c r="P3" s="18">
         <f>(1+Q3)^(12)-1</f>
-        <v>0.38158127377921258</v>
+        <v>1.7401841997915479</v>
       </c>
       <c r="Q3" s="22">
         <f>IRR(I2:I74)</f>
-        <v>2.7301770284872129E-2</v>
+        <v>8.763117278725896E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -5609,18 +5609,18 @@
       </c>
       <c r="K4" s="6">
         <f>K3+J4</f>
-        <v>2533.6225551394091</v>
+        <v>1047883.2372826176</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L67" si="0">K4*B4</f>
-        <v>2052.2342696629216</v>
+        <v>848785.42219892028</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>18</v>
       </c>
       <c r="P4" s="19">
         <f>NPV(Q5,I2:I74)</f>
-        <v>78164.244666387211</v>
+        <v>2874971.2253880636</v>
       </c>
       <c r="Q4" s="24"/>
     </row>
@@ -5657,11 +5657,11 @@
       </c>
       <c r="K5" s="6">
         <f t="shared" ref="K5:K68" si="1">K4+J5</f>
-        <v>3459.5484810653352</v>
+        <v>1048809.1632085436</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="0"/>
-        <v>2802.2342696629216</v>
+        <v>849535.42219892028</v>
       </c>
       <c r="O5" s="12" t="s">
         <v>20</v>
@@ -5707,11 +5707,11 @@
       </c>
       <c r="K6" s="6">
         <f t="shared" si="1"/>
-        <v>4331.6415043211491</v>
+        <v>1049681.2562317993</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="0"/>
-        <v>3725.2116937161882</v>
+        <v>902725.88035934733</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -5747,11 +5747,11 @@
       </c>
       <c r="K7" s="6">
         <f t="shared" si="1"/>
-        <v>5121.1151885316758</v>
+        <v>1050470.7299160098</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="0"/>
-        <v>4865.059429105092</v>
+        <v>997947.19342020922</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -5787,11 +5787,11 @@
       </c>
       <c r="K8" s="6">
         <f t="shared" si="1"/>
-        <v>5918.9875289572083</v>
+        <v>1051268.6022564354</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="0"/>
-        <v>5563.8482772197758</v>
+        <v>988192.48612104927</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -5827,11 +5827,11 @@
       </c>
       <c r="K9" s="6">
         <f t="shared" si="1"/>
-        <v>6761.6841581706913</v>
+        <v>1052111.2988856488</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="0"/>
-        <v>6017.8989007719156</v>
+        <v>936379.05600822752</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -5867,11 +5867,11 @@
       </c>
       <c r="K10" s="6">
         <f t="shared" si="1"/>
-        <v>7723.2226197091532</v>
+        <v>1053072.8373471873</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="0"/>
-        <v>6024.1136433731399</v>
+        <v>821396.8131308062</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -5907,11 +5907,11 @@
       </c>
       <c r="K11" s="6">
         <f t="shared" si="1"/>
-        <v>8750.6198799831254</v>
+        <v>1054100.2346074614</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="0"/>
-        <v>6387.9525123876811</v>
+        <v>769493.1712634468</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -5947,11 +5947,11 @@
       </c>
       <c r="K12" s="6">
         <f t="shared" si="1"/>
-        <v>9724.6458540090989</v>
+        <v>1055074.2605814873</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="0"/>
-        <v>7487.9773075870062</v>
+        <v>812407.18064774526</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -5987,11 +5987,11 @@
       </c>
       <c r="K13" s="6">
         <f t="shared" si="1"/>
-        <v>10628.260311840424</v>
+        <v>1055977.8750393186</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="0"/>
-        <v>8821.4560588275508</v>
+        <v>876461.63628263434</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -6027,11 +6027,11 @@
       </c>
       <c r="K14" s="6">
         <f t="shared" si="1"/>
-        <v>11417.733996050951</v>
+        <v>1056767.3487235291</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>10846.847296248403</v>
+        <v>1003928.9812873526</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -6067,11 +6067,11 @@
       </c>
       <c r="K15" s="6">
         <f t="shared" si="1"/>
-        <v>12118.668575490203</v>
+        <v>1057468.2833029684</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="0"/>
-        <v>12966.975375774518</v>
+        <v>1131491.0631341762</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -6107,11 +6107,11 @@
       </c>
       <c r="K16" s="6">
         <f t="shared" si="1"/>
-        <v>12868.668575490203</v>
+        <v>1058218.2833029684</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="0"/>
-        <v>12868.668575490203</v>
+        <v>1058218.2833029684</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -6147,11 +6147,11 @@
       </c>
       <c r="K17" s="6">
         <f t="shared" si="1"/>
-        <v>13658.142259700729</v>
+        <v>1059007.7569871789</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" si="0"/>
-        <v>12975.235146715693</v>
+        <v>1006057.36913782</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -6187,11 +6187,11 @@
       </c>
       <c r="K18" s="6">
         <f t="shared" si="1"/>
-        <v>14595.642259700729</v>
+        <v>1059945.2569871789</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="0"/>
-        <v>11676.513807760584</v>
+        <v>847956.20558974321</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -6227,11 +6227,11 @@
       </c>
       <c r="K19" s="6">
         <f t="shared" si="1"/>
-        <v>15582.484364963888</v>
+        <v>1060932.0990924421</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="0"/>
-        <v>11842.688117372554</v>
+        <v>806308.39531025593</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -6267,11 +6267,11 @@
       </c>
       <c r="K20" s="6">
         <f t="shared" si="1"/>
-        <v>16624.151031630554</v>
+        <v>1061973.7657591088</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="0"/>
-        <v>11969.388742773999</v>
+        <v>764621.11134655832</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -6307,11 +6307,11 @@
       </c>
       <c r="K21" s="6">
         <f t="shared" si="1"/>
-        <v>17538.785177972019</v>
+        <v>1062888.3999054502</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="0"/>
-        <v>14381.803845937055</v>
+        <v>871568.48792246904</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -6347,11 +6347,11 @@
       </c>
       <c r="K22" s="6">
         <f t="shared" si="1"/>
-        <v>18488.152266579615</v>
+        <v>1063837.7669940577</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="0"/>
-        <v>14605.640290597896</v>
+        <v>840431.83592530561</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -6387,11 +6387,11 @@
       </c>
       <c r="K23" s="6">
         <f t="shared" si="1"/>
-        <v>19449.690728118076</v>
+        <v>1064799.3054555962</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="0"/>
-        <v>15170.758767932099</v>
+        <v>830543.45825536503</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -6427,11 +6427,11 @@
       </c>
       <c r="K24" s="6">
         <f t="shared" si="1"/>
-        <v>20399.057816725672</v>
+        <v>1065748.6725442037</v>
       </c>
       <c r="L24" s="4">
         <f t="shared" si="0"/>
-        <v>16115.25567521328</v>
+        <v>841941.45130992099</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -6467,11 +6467,11 @@
       </c>
       <c r="K25" s="6">
         <f t="shared" si="1"/>
-        <v>21412.571330239185</v>
+        <v>1066762.1860577173</v>
       </c>
       <c r="L25" s="4">
         <f t="shared" si="0"/>
-        <v>15845.302784376996</v>
+        <v>789404.01768271078</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -6507,11 +6507,11 @@
       </c>
       <c r="K26" s="6">
         <f t="shared" si="1"/>
-        <v>22454.237996905853</v>
+        <v>1067803.8527243841</v>
       </c>
       <c r="L26" s="4">
         <f t="shared" si="0"/>
-        <v>16167.051357772214</v>
+        <v>768818.77396155649</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -6547,11 +6547,11 @@
       </c>
       <c r="K27" s="6">
         <f t="shared" si="1"/>
-        <v>23441.080102169009</v>
+        <v>1068790.6948296472</v>
       </c>
       <c r="L27" s="4">
         <f t="shared" si="0"/>
-        <v>17815.220877648448</v>
+        <v>812280.92807053193</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -6587,11 +6587,11 @@
       </c>
       <c r="K28" s="6">
         <f t="shared" si="1"/>
-        <v>24183.654359594751</v>
+        <v>1069533.2690870729</v>
       </c>
       <c r="L28" s="4">
         <f t="shared" si="0"/>
-        <v>24425.490903190701</v>
+        <v>1080228.6017779438</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -6627,11 +6627,11 @@
       </c>
       <c r="K29" s="6">
         <f t="shared" si="1"/>
-        <v>24998.871750899099</v>
+        <v>1070348.4864783774</v>
       </c>
       <c r="L29" s="4">
         <f t="shared" si="0"/>
-        <v>22998.962010827174</v>
+        <v>984720.60756010725</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -6667,11 +6667,11 @@
       </c>
       <c r="K30" s="6">
         <f t="shared" si="1"/>
-        <v>25814.089142203447</v>
+        <v>1071163.7038696818</v>
       </c>
       <c r="L30" s="4">
         <f t="shared" si="0"/>
-        <v>23748.962010827174</v>
+        <v>985470.60756010725</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -6707,11 +6707,11 @@
       </c>
       <c r="K31" s="6">
         <f t="shared" si="1"/>
-        <v>26495.907324021628</v>
+        <v>1071845.5220514999</v>
       </c>
       <c r="L31" s="4">
         <f t="shared" si="0"/>
-        <v>29145.498056423792</v>
+        <v>1179030.0742566499</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -6747,11 +6747,11 @@
       </c>
       <c r="K32" s="6">
         <f t="shared" si="1"/>
-        <v>27245.907324021628</v>
+        <v>1072595.5220514999</v>
       </c>
       <c r="L32" s="4">
         <f t="shared" si="0"/>
-        <v>27245.907324021628</v>
+        <v>1072595.5220514999</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -6787,11 +6787,11 @@
       </c>
       <c r="K33" s="6">
         <f t="shared" si="1"/>
-        <v>27860.661422382283</v>
+        <v>1073210.2761498606</v>
       </c>
       <c r="L33" s="4">
         <f t="shared" si="0"/>
-        <v>33990.006935306388</v>
+        <v>1309316.5369028298</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -6827,11 +6827,11 @@
       </c>
       <c r="K34" s="6">
         <f t="shared" si="1"/>
-        <v>28530.304279525142</v>
+        <v>1073879.9190070035</v>
       </c>
       <c r="L34" s="4">
         <f t="shared" si="0"/>
-        <v>31953.940793068163</v>
+        <v>1202745.5092878442</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -6867,11 +6867,11 @@
       </c>
       <c r="K35" s="6">
         <f t="shared" si="1"/>
-        <v>29188.199016367249</v>
+        <v>1074537.8137438456</v>
       </c>
       <c r="L35" s="4">
         <f t="shared" si="0"/>
-        <v>33274.546878658664</v>
+        <v>1224973.1076679837</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -6907,11 +6907,11 @@
       </c>
       <c r="K36" s="6">
         <f t="shared" si="1"/>
-        <v>29986.071356792781</v>
+        <v>1075335.6860842712</v>
       </c>
       <c r="L36" s="4">
         <f t="shared" si="0"/>
-        <v>28186.907075385214</v>
+        <v>1010815.5449192148</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -6947,11 +6947,11 @@
       </c>
       <c r="K37" s="6">
         <f t="shared" si="1"/>
-        <v>30751.377479241761</v>
+        <v>1076100.9922067202</v>
       </c>
       <c r="L37" s="4">
         <f t="shared" si="0"/>
-        <v>30136.349929656924</v>
+        <v>1054578.9723625858</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -6987,11 +6987,11 @@
       </c>
       <c r="K38" s="6">
         <f t="shared" si="1"/>
-        <v>31397.929203379692</v>
+        <v>1076747.5439308581</v>
       </c>
       <c r="L38" s="4">
         <f t="shared" si="0"/>
-        <v>36421.597875920437</v>
+        <v>1249027.1509597953</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -7027,11 +7027,11 @@
       </c>
       <c r="K39" s="6">
         <f t="shared" si="1"/>
-        <v>31953.484758935247</v>
+        <v>1077303.0994864136</v>
       </c>
       <c r="L39" s="4">
         <f t="shared" si="0"/>
-        <v>43137.204424562588</v>
+        <v>1454359.1843066586</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -7067,11 +7067,11 @@
       </c>
       <c r="K40" s="6">
         <f t="shared" si="1"/>
-        <v>32611.379495777353</v>
+        <v>1077960.9942232557</v>
       </c>
       <c r="L40" s="4">
         <f t="shared" si="0"/>
-        <v>37176.972625186179</v>
+        <v>1228875.5334145112</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -7107,11 +7107,11 @@
       </c>
       <c r="K41" s="6">
         <f t="shared" si="1"/>
-        <v>33179.561313959173</v>
+        <v>1078529.1760414375</v>
       </c>
       <c r="L41" s="4">
         <f t="shared" si="0"/>
-        <v>43797.020934426109</v>
+        <v>1423658.5123746977</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -7147,11 +7147,11 @@
       </c>
       <c r="K42" s="6">
         <f t="shared" si="1"/>
-        <v>33689.765395591829</v>
+        <v>1079039.3801230702</v>
       </c>
       <c r="L42" s="4">
         <f t="shared" si="0"/>
-        <v>49523.955131519986</v>
+        <v>1586187.8887809131</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -7187,11 +7187,11 @@
       </c>
       <c r="K43" s="6">
         <f t="shared" si="1"/>
-        <v>34128.361886819897</v>
+        <v>1079477.9766142983</v>
       </c>
       <c r="L43" s="4">
         <f t="shared" si="0"/>
-        <v>58359.498826462026</v>
+        <v>1845907.34001045</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -7227,11 +7227,11 @@
       </c>
       <c r="K44" s="6">
         <f t="shared" si="1"/>
-        <v>34580.16911573556</v>
+        <v>1079929.7838432139</v>
       </c>
       <c r="L44" s="4">
         <f t="shared" si="0"/>
-        <v>57403.080732121023</v>
+        <v>1792683.4411797351</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -7267,11 +7267,11 @@
       </c>
       <c r="K45" s="6">
         <f t="shared" si="1"/>
-        <v>35243.885929894852</v>
+        <v>1080593.5006573731</v>
       </c>
       <c r="L45" s="4">
         <f t="shared" si="0"/>
-        <v>39825.591100781181</v>
+        <v>1221070.6557428315</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -7307,11 +7307,11 @@
       </c>
       <c r="K46" s="6">
         <f t="shared" si="1"/>
-        <v>35925.704111713036</v>
+        <v>1081275.3188391912</v>
       </c>
       <c r="L46" s="4">
         <f t="shared" si="0"/>
-        <v>39518.274522884341</v>
+        <v>1189402.8507231104</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -7347,11 +7347,11 @@
       </c>
       <c r="K47" s="6">
         <f t="shared" si="1"/>
-        <v>36469.182372582603</v>
+        <v>1081818.7971000609</v>
       </c>
       <c r="L47" s="4">
         <f t="shared" si="0"/>
-        <v>50327.471674163986</v>
+        <v>1492909.9399980837</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -7387,11 +7387,11 @@
       </c>
       <c r="K48" s="6">
         <f t="shared" si="1"/>
-        <v>37204.476490229659</v>
+        <v>1082554.0912177078</v>
       </c>
       <c r="L48" s="4">
         <f t="shared" si="0"/>
-        <v>37948.566020034254</v>
+        <v>1104205.173042062</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -7427,11 +7427,11 @@
       </c>
       <c r="K49" s="6">
         <f t="shared" si="1"/>
-        <v>37814.232587790633</v>
+        <v>1083163.8473152688</v>
       </c>
       <c r="L49" s="4">
         <f t="shared" si="0"/>
-        <v>46511.50608298248</v>
+        <v>1332291.5321977807</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -7467,11 +7467,11 @@
       </c>
       <c r="K50" s="6">
         <f t="shared" si="1"/>
-        <v>38400.170087790633</v>
+        <v>1083749.7848152688</v>
       </c>
       <c r="L50" s="4">
         <f t="shared" si="0"/>
-        <v>49152.21771237201</v>
+        <v>1387199.7245635442</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -7507,11 +7507,11 @@
       </c>
       <c r="K51" s="6">
         <f t="shared" si="1"/>
-        <v>39000.170087790633</v>
+        <v>1084349.7848152688</v>
       </c>
       <c r="L51" s="4">
         <f t="shared" si="0"/>
-        <v>48750.212609738293</v>
+        <v>1355437.231019086</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -7547,11 +7547,11 @@
       </c>
       <c r="K52" s="6">
         <f t="shared" si="1"/>
-        <v>39614.924186151286</v>
+        <v>1084964.5389136295</v>
       </c>
       <c r="L52" s="4">
         <f t="shared" si="0"/>
-        <v>48330.207507104569</v>
+        <v>1323656.737474628</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -7587,11 +7587,11 @@
       </c>
       <c r="K53" s="6">
         <f t="shared" si="1"/>
-        <v>40229.678284511938</v>
+        <v>1085579.2930119901</v>
       </c>
       <c r="L53" s="4">
         <f t="shared" si="0"/>
-        <v>49080.207507104562</v>
+        <v>1324406.737474628</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -7627,11 +7627,11 @@
       </c>
       <c r="K54" s="6">
         <f t="shared" si="1"/>
-        <v>40789.379777049253</v>
+        <v>1086138.9945045274</v>
       </c>
       <c r="L54" s="4">
         <f t="shared" si="0"/>
-        <v>54657.768901246003</v>
+        <v>1455426.2526360669</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -7667,11 +7667,11 @@
       </c>
       <c r="K55" s="6">
         <f t="shared" si="1"/>
-        <v>41255.21828636602</v>
+        <v>1086604.8330138442</v>
       </c>
       <c r="L55" s="4">
         <f t="shared" si="0"/>
-        <v>66420.901441049296</v>
+        <v>1749433.7811522894</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -7707,11 +7707,11 @@
       </c>
       <c r="K56" s="6">
         <f t="shared" si="1"/>
-        <v>41641.816224510352</v>
+        <v>1086991.4309519886</v>
       </c>
       <c r="L56" s="4">
         <f t="shared" si="0"/>
-        <v>80785.123475550077</v>
+        <v>2108763.3760468578</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -7747,11 +7747,11 @@
       </c>
       <c r="K57" s="6">
         <f t="shared" si="1"/>
-        <v>42093.623453426015</v>
+        <v>1087443.2381809042</v>
       </c>
       <c r="L57" s="4">
         <f t="shared" si="0"/>
-        <v>69875.414932687185</v>
+        <v>1805155.7753803008</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -7787,11 +7787,11 @@
       </c>
       <c r="K58" s="6">
         <f t="shared" si="1"/>
-        <v>42510.290120092679</v>
+        <v>1087859.9048475709</v>
       </c>
       <c r="L58" s="4">
         <f t="shared" si="0"/>
-        <v>76518.522216166821</v>
+        <v>1958147.8287256276</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -7827,11 +7827,11 @@
       </c>
       <c r="K59" s="6">
         <f t="shared" si="1"/>
-        <v>42892.943181317169</v>
+        <v>1088242.5579087953</v>
       </c>
       <c r="L59" s="4">
         <f t="shared" si="0"/>
-        <v>84070.168635381648</v>
+        <v>2132955.4135012389</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -7867,11 +7867,11 @@
       </c>
       <c r="K60" s="6">
         <f t="shared" si="1"/>
-        <v>43262.401309395987</v>
+        <v>1088612.0160368741</v>
       </c>
       <c r="L60" s="4">
         <f t="shared" si="0"/>
-        <v>87822.67465807384</v>
+        <v>2209882.3925548545</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -7907,11 +7907,11 @@
       </c>
       <c r="K61" s="6">
         <f t="shared" si="1"/>
-        <v>43576.208840776744</v>
+        <v>1088925.8235682549</v>
       </c>
       <c r="L61" s="4">
         <f t="shared" si="0"/>
-        <v>104147.13912945642</v>
+        <v>2602532.7183281295</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -7947,11 +7947,11 @@
       </c>
       <c r="K62" s="6">
         <f t="shared" si="1"/>
-        <v>43817.366397046841</v>
+        <v>1089166.981124525</v>
       </c>
       <c r="L62" s="4">
         <f t="shared" si="0"/>
-        <v>136272.00949481566</v>
+        <v>3387309.3112972723</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -7987,11 +7987,11 @@
       </c>
       <c r="K63" s="6">
         <f t="shared" si="1"/>
-        <v>44063.268036391106</v>
+        <v>1089412.8827638691</v>
       </c>
       <c r="L63" s="4">
         <f t="shared" si="0"/>
-        <v>134392.96751099286</v>
+        <v>3322709.2924298006</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -8027,11 +8027,11 @@
       </c>
       <c r="K64" s="6">
         <f t="shared" si="1"/>
-        <v>44352.843325966394</v>
+        <v>1089702.4580534445</v>
       </c>
       <c r="L64" s="4">
         <f t="shared" si="0"/>
-        <v>114873.86421425296</v>
+        <v>2822329.3663584213</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -8067,11 +8067,11 @@
       </c>
       <c r="K65" s="6">
         <f t="shared" si="1"/>
-        <v>44625.570598693666</v>
+        <v>1089975.1853261718</v>
       </c>
       <c r="L65" s="4">
         <f t="shared" si="0"/>
-        <v>122720.31914640758</v>
+        <v>2997431.7596469726</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -8107,11 +8107,11 @@
       </c>
       <c r="K66" s="6">
         <f t="shared" si="1"/>
-        <v>44878.948977072047</v>
+        <v>1090228.5637045503</v>
       </c>
       <c r="L66" s="4">
         <f t="shared" si="0"/>
-        <v>132841.68897213327</v>
+        <v>3227076.5485654688</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -8147,11 +8147,11 @@
       </c>
       <c r="K67" s="6">
         <f t="shared" si="1"/>
-        <v>45187.590952380691</v>
+        <v>1090537.2056798588</v>
       </c>
       <c r="L67" s="4">
         <f t="shared" si="0"/>
-        <v>109805.84601428508</v>
+        <v>2650005.4098020568</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -8187,11 +8187,11 @@
       </c>
       <c r="K68" s="6">
         <f t="shared" si="1"/>
-        <v>45471.681861471603</v>
+        <v>1090821.2965889496</v>
       </c>
       <c r="L68" s="4">
         <f t="shared" ref="L68:L73" si="2">K68*B68</f>
-        <v>120045.24011428504</v>
+        <v>2879768.2229948272</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -8227,11 +8227,11 @@
       </c>
       <c r="K69" s="6">
         <f t="shared" ref="K69:K73" si="3">K68+J69</f>
-        <v>45733.919623709364</v>
+        <v>1091083.5343511873</v>
       </c>
       <c r="L69" s="4">
         <f t="shared" si="2"/>
-        <v>130799.01012380878</v>
+        <v>3120498.9082443956</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -8267,11 +8267,11 @@
       </c>
       <c r="K70" s="6">
         <f t="shared" si="3"/>
-        <v>45990.768938777859</v>
+        <v>1091340.3836662557</v>
       </c>
       <c r="L70" s="4">
         <f t="shared" si="2"/>
-        <v>134293.04530123135</v>
+        <v>3186713.9203054667</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -8307,11 +8307,11 @@
       </c>
       <c r="K71" s="6">
         <f t="shared" si="3"/>
-        <v>46234.275432284354</v>
+        <v>1091583.8901597622</v>
       </c>
       <c r="L71" s="4">
         <f t="shared" si="2"/>
-        <v>142401.56833143582</v>
+        <v>3362078.3816920677</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -8347,11 +8347,11 @@
       </c>
       <c r="K72" s="6">
         <f t="shared" si="3"/>
-        <v>46468.650432284354</v>
+        <v>1091818.2651597622</v>
       </c>
       <c r="L72" s="4">
         <f t="shared" si="2"/>
-        <v>148699.68138330994</v>
+        <v>3493818.4485112391</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -8387,17 +8387,17 @@
       </c>
       <c r="K73" s="6">
         <f t="shared" si="3"/>
-        <v>46676.98376561769</v>
+        <v>1092026.5984930955</v>
       </c>
       <c r="L73" s="4">
         <f t="shared" si="2"/>
-        <v>168037.14155622368</v>
+        <v>3931295.754575144</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="I74" s="4">
         <f>L73</f>
-        <v>168037.14155622368</v>
+        <v>3931295.754575144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>